<commit_message>
Initial progress on improving classifier
</commit_message>
<xml_diff>
--- a/documentation/functional_requirements.xlsx
+++ b/documentation/functional_requirements.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ThomasFranklin/Tweet-Classification/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189C47B-88A8-EC4D-A35E-257FCCB42234}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074BF50-C62B-FC44-8419-1F0500C0A2DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14960" xr2:uid="{56A7DCBB-48D4-8C4C-8F17-FD744938F507}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -549,7 +549,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F13" sqref="F3:F13"/>
     </sheetView>
   </sheetViews>
@@ -631,29 +631,29 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <f>(C3*C$1)+D3*D$1</f>
+        <f t="shared" ref="E3:E16" si="0">(C3*C$1)+D3*D$1</f>
         <v>27</v>
       </c>
       <c r="F3" s="2">
-        <f>ROUND(E3/E$17,2)</f>
+        <f t="shared" ref="F3:F16" si="1">ROUND(E3/E$17,2)</f>
         <v>0.09</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
       </c>
       <c r="H3" s="2">
-        <f>ROUND(G3/G$17,2)</f>
+        <f t="shared" ref="H3:H16" si="2">ROUND(G3/G$17,2)</f>
         <v>0.09</v>
       </c>
       <c r="I3" s="2">
         <v>4</v>
       </c>
       <c r="J3" s="2">
-        <f>ROUND(I3/I$17,2)</f>
+        <f t="shared" ref="J3:J16" si="3">ROUND(I3/I$17,2)</f>
         <v>0.06</v>
       </c>
       <c r="K3" s="2">
-        <f>ROUND((F3)/(H3*0+J3*I$1),2)</f>
+        <f t="shared" ref="K3:K16" si="4">ROUND((F3)/(H3*0+J3*I$1),2)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -671,29 +671,29 @@
         <v>2</v>
       </c>
       <c r="E4" s="2">
-        <f>(C4*C$1)+D4*D$1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F4" s="2">
-        <f>ROUND(E4/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
       </c>
       <c r="H4" s="2">
-        <f>ROUND(G4/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="I4" s="2">
         <v>3</v>
       </c>
       <c r="J4" s="2">
-        <f>ROUND(I4/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K4" s="2">
-        <f>ROUND((F4)/(H4*0+J4*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
     </row>
@@ -711,29 +711,29 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>(C5*C$1)+D5*D$1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F5" s="2">
-        <f>ROUND(E5/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G5" s="2">
         <v>9</v>
       </c>
       <c r="H5" s="2">
-        <f>ROUND(G5/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I5" s="2">
         <v>6</v>
       </c>
       <c r="J5" s="2">
-        <f>ROUND(I5/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="K5" s="2">
-        <f>ROUND((F5)/(H5*0+J5*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -751,29 +751,29 @@
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <f>(C6*C$1)+D6*D$1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F6" s="2">
-        <f>ROUND(E6/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="G6" s="2">
         <v>3</v>
       </c>
       <c r="H6" s="2">
-        <f>ROUND(G6/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="I6" s="2">
         <v>3</v>
       </c>
       <c r="J6" s="2">
-        <f>ROUND(I6/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K6" s="2">
-        <f>ROUND((F6)/(H6*0+J6*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
     </row>
@@ -791,29 +791,29 @@
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <f>(C7*C$1)+D7*D$1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F7" s="2">
-        <f>ROUND(E7/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="G7" s="2">
         <v>3</v>
       </c>
       <c r="H7" s="2">
-        <f>ROUND(G7/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="I7" s="2">
         <v>3</v>
       </c>
       <c r="J7" s="2">
-        <f>ROUND(I7/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K7" s="2">
-        <f>ROUND((F7)/(H7*0+J7*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
     </row>
@@ -831,29 +831,29 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <f>(C8*C$1)+D8*D$1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F8" s="2">
-        <f>ROUND(E8/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G8" s="2">
         <v>9</v>
       </c>
       <c r="H8" s="2">
-        <f>ROUND(G8/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
       </c>
       <c r="J8" s="2">
-        <f>ROUND(I8/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="K8" s="2">
-        <f>ROUND((F8)/(H8*0+J8*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.39</v>
       </c>
     </row>
@@ -871,29 +871,29 @@
         <v>9</v>
       </c>
       <c r="E9" s="2">
-        <f>(C9*C$1)+D9*D$1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F9" s="2">
-        <f>ROUND(E9/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="G9" s="2">
         <v>3</v>
       </c>
       <c r="H9" s="2">
-        <f>ROUND(G9/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="I9" s="2">
         <v>3</v>
       </c>
       <c r="J9" s="2">
-        <f>ROUND(I9/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K9" s="2">
-        <f>ROUND((F9)/(H9*0+J9*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
     </row>
@@ -911,29 +911,29 @@
         <v>9</v>
       </c>
       <c r="E10" s="2">
-        <f>(C10*C$1)+D10*D$1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F10" s="2">
-        <f>ROUND(E10/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="G10" s="2">
         <v>3</v>
       </c>
       <c r="H10" s="2">
-        <f>ROUND(G10/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="I10" s="2">
         <v>3</v>
       </c>
       <c r="J10" s="2">
-        <f>ROUND(I10/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K10" s="2">
-        <f>ROUND((F10)/(H10*0+J10*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
     </row>
@@ -951,29 +951,29 @@
         <v>3</v>
       </c>
       <c r="E11" s="2">
-        <f>(C11*C$1)+D11*D$1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F11" s="2">
-        <f>ROUND(E11/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G11" s="2">
         <v>9</v>
       </c>
       <c r="H11" s="2">
-        <f>ROUND(G11/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I11" s="2">
         <v>7</v>
       </c>
       <c r="J11" s="2">
-        <f>ROUND(I11/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="K11" s="2">
-        <f>ROUND((F11)/(H11*0+J11*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
     </row>
@@ -991,29 +991,29 @@
         <v>6</v>
       </c>
       <c r="E12" s="2">
-        <f>(C12*C$1)+D12*D$1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F12" s="2">
-        <f>ROUND(E12/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <f>ROUND(G12/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
       <c r="I12" s="2">
         <v>3</v>
       </c>
       <c r="J12" s="2">
-        <f>ROUND(I12/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="K12" s="2">
-        <f>ROUND((F12)/(H12*0+J12*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -1031,29 +1031,29 @@
         <v>3</v>
       </c>
       <c r="E13" s="2">
-        <f>(C13*C$1)+D13*D$1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F13" s="2">
-        <f>ROUND(E13/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G13" s="2">
         <v>9</v>
       </c>
       <c r="H13" s="2">
-        <f>ROUND(G13/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I13" s="2">
         <v>6</v>
       </c>
       <c r="J13" s="2">
-        <f>ROUND(I13/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="K13" s="2">
-        <f>ROUND((F13)/(H13*0+J13*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -1071,29 +1071,29 @@
         <v>9</v>
       </c>
       <c r="E14" s="2">
-        <f>(C14*C$1)+D14*D$1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F14" s="2">
-        <f>ROUND(E14/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G14" s="2">
         <v>9</v>
       </c>
       <c r="H14" s="2">
-        <f>ROUND(G14/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I14" s="2">
         <v>7</v>
       </c>
       <c r="J14" s="2">
-        <f>ROUND(I14/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="K14" s="2">
-        <f>ROUND((F14)/(H14*0+J14*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
     </row>
@@ -1111,29 +1111,29 @@
         <v>9</v>
       </c>
       <c r="E15" s="2">
-        <f>(C15*C$1)+D15*D$1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F15" s="2">
-        <f>ROUND(E15/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G15" s="2">
         <v>9</v>
       </c>
       <c r="H15" s="2">
-        <f>ROUND(G15/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
       <c r="I15" s="2">
         <v>7</v>
       </c>
       <c r="J15" s="2">
-        <f>ROUND(I15/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="K15" s="2">
-        <f>ROUND((F15)/(H15*0+J15*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
       <c r="O15" s="6"/>
@@ -1154,29 +1154,29 @@
         <v>9</v>
       </c>
       <c r="E16" s="2">
-        <f>(C16*C$1)+D16*D$1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F16" s="2">
-        <f>ROUND(E16/E$17,2)</f>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
       <c r="H16" s="2">
-        <f>ROUND(G16/G$17,2)</f>
+        <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
       <c r="I16" s="2">
         <v>4</v>
       </c>
       <c r="J16" s="2">
-        <f>ROUND(I16/I$17,2)</f>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="K16" s="2">
-        <f>ROUND((F16)/(H16*0+J16*I$1),2)</f>
+        <f t="shared" si="4"/>
         <v>0.67</v>
       </c>
       <c r="O16" s="6"/>

</xml_diff>